<commit_message>
Changed project file gor economics section
</commit_message>
<xml_diff>
--- a/Documentation/Длительность работ.xlsx
+++ b/Documentation/Длительность работ.xlsx
@@ -429,16 +429,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>595887.5</c:v>
+                  <c:v>508250</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>97800</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>357532.5</c:v>
+                  <c:v>304950</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>58800</c:v>
+                  <c:v>39200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1416,7 +1416,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1487,7 +1487,7 @@
         <v>16</v>
       </c>
       <c r="H4">
-        <v>595887.5</v>
+        <v>508250</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
@@ -1527,7 +1527,7 @@
         <v>18</v>
       </c>
       <c r="H6">
-        <v>357532.5</v>
+        <v>304950</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
@@ -1547,7 +1547,7 @@
         <v>19</v>
       </c>
       <c r="H7">
-        <v>58800</v>
+        <v>39200</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">

</xml_diff>